<commit_message>
fixed document generation and rest api. Removed debugging from cards in the staff url
</commit_message>
<xml_diff>
--- a/excel/transfer.xlsx
+++ b/excel/transfer.xlsx
@@ -1730,21 +1730,11 @@
       <c r="Q4" s="1" t="n"/>
     </row>
     <row r="5" ht="16.5" customHeight="1">
-      <c r="A5" s="15" t="inlineStr">
-        <is>
-          <t>GL 501</t>
-        </is>
-      </c>
-      <c r="B5" s="51" t="inlineStr">
-        <is>
-          <t>08:45</t>
-        </is>
-      </c>
+      <c r="A5" s="15" t="inlineStr"/>
+      <c r="B5" s="51" t="inlineStr"/>
       <c r="C5" s="150" t="inlineStr"/>
       <c r="D5" s="151" t="n"/>
-      <c r="E5" s="64" t="n">
-        <v>0</v>
-      </c>
+      <c r="E5" s="64" t="inlineStr"/>
       <c r="F5" s="55" t="n"/>
       <c r="G5" s="53" t="n"/>
       <c r="H5" s="152" t="n"/>
@@ -1753,25 +1743,11 @@
       <c r="Q5" s="1" t="n"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="15" t="inlineStr">
-        <is>
-          <t>GL 533</t>
-        </is>
-      </c>
-      <c r="B6" s="59" t="inlineStr">
-        <is>
-          <t>11:10</t>
-        </is>
-      </c>
-      <c r="C6" s="153" t="inlineStr">
-        <is>
-          <t>2;</t>
-        </is>
-      </c>
+      <c r="A6" s="15" t="inlineStr"/>
+      <c r="B6" s="59" t="inlineStr"/>
+      <c r="C6" s="153" t="inlineStr"/>
       <c r="D6" s="151" t="n"/>
-      <c r="E6" s="25" t="n">
-        <v>1</v>
-      </c>
+      <c r="E6" s="25" t="inlineStr"/>
       <c r="F6" s="52" t="n"/>
       <c r="G6" s="50" t="n"/>
       <c r="H6" s="154" t="n"/>
@@ -1780,25 +1756,11 @@
       <c r="Q6" s="1" t="n"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="15" t="inlineStr">
-        <is>
-          <t>GL 571</t>
-        </is>
-      </c>
-      <c r="B7" s="51" t="inlineStr">
-        <is>
-          <t>11:40</t>
-        </is>
-      </c>
-      <c r="C7" s="155" t="inlineStr">
-        <is>
-          <t>2;</t>
-        </is>
-      </c>
+      <c r="A7" s="15" t="inlineStr"/>
+      <c r="B7" s="51" t="inlineStr"/>
+      <c r="C7" s="155" t="inlineStr"/>
       <c r="D7" s="151" t="n"/>
-      <c r="E7" s="25" t="n">
-        <v>1</v>
-      </c>
+      <c r="E7" s="25" t="inlineStr"/>
       <c r="F7" s="52" t="n"/>
       <c r="G7" s="50" t="n"/>
       <c r="H7" s="154" t="n"/>
@@ -1808,25 +1770,11 @@
       <c r="Q7" s="1" t="n"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="15" t="inlineStr">
-        <is>
-          <t>GL 8575</t>
-        </is>
-      </c>
-      <c r="B8" s="51" t="inlineStr">
-        <is>
-          <t>13:25</t>
-        </is>
-      </c>
-      <c r="C8" s="155" t="inlineStr">
-        <is>
-          <t>2;2;</t>
-        </is>
-      </c>
+      <c r="A8" s="15" t="inlineStr"/>
+      <c r="B8" s="51" t="inlineStr"/>
+      <c r="C8" s="155" t="inlineStr"/>
       <c r="D8" s="151" t="n"/>
-      <c r="E8" s="64" t="n">
-        <v>2</v>
-      </c>
+      <c r="E8" s="64" t="inlineStr"/>
       <c r="F8" s="21" t="n"/>
       <c r="G8" s="50" t="n"/>
       <c r="H8" s="154" t="n"/>
@@ -1836,11 +1784,11 @@
       <c r="Q8" s="1" t="n"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="15" t="n"/>
-      <c r="B9" s="51" t="n"/>
-      <c r="C9" s="49" t="n"/>
+      <c r="A9" s="15" t="inlineStr"/>
+      <c r="B9" s="51" t="inlineStr"/>
+      <c r="C9" s="49" t="inlineStr"/>
       <c r="D9" s="151" t="n"/>
-      <c r="E9" s="64" t="n"/>
+      <c r="E9" s="64" t="inlineStr"/>
       <c r="F9" s="20" t="n"/>
       <c r="G9" s="50" t="n"/>
       <c r="H9" s="154" t="n"/>
@@ -1850,11 +1798,11 @@
       <c r="Q9" s="1" t="n"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="15" t="n"/>
-      <c r="B10" s="51" t="n"/>
-      <c r="C10" s="155" t="n"/>
+      <c r="A10" s="15" t="inlineStr"/>
+      <c r="B10" s="51" t="inlineStr"/>
+      <c r="C10" s="155" t="inlineStr"/>
       <c r="D10" s="151" t="n"/>
-      <c r="E10" s="64" t="n"/>
+      <c r="E10" s="64" t="inlineStr"/>
       <c r="F10" s="20" t="n"/>
       <c r="G10" s="50" t="n"/>
       <c r="H10" s="156" t="n"/>
@@ -1864,11 +1812,11 @@
       <c r="Q10" s="1" t="n"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="15" t="n"/>
-      <c r="B11" s="51" t="n"/>
-      <c r="C11" s="155" t="n"/>
+      <c r="A11" s="15" t="inlineStr"/>
+      <c r="B11" s="51" t="inlineStr"/>
+      <c r="C11" s="155" t="inlineStr"/>
       <c r="D11" s="151" t="n"/>
-      <c r="E11" s="64" t="n"/>
+      <c r="E11" s="64" t="inlineStr"/>
       <c r="F11" s="20" t="n"/>
       <c r="G11" s="50" t="n"/>
       <c r="H11" s="156" t="n"/>
@@ -1879,11 +1827,11 @@
       <c r="R11" s="1" t="n"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="15" t="n"/>
-      <c r="B12" s="51" t="n"/>
-      <c r="C12" s="49" t="n"/>
+      <c r="A12" s="15" t="inlineStr"/>
+      <c r="B12" s="51" t="inlineStr"/>
+      <c r="C12" s="49" t="inlineStr"/>
       <c r="D12" s="151" t="n"/>
-      <c r="E12" s="64" t="n"/>
+      <c r="E12" s="64" t="inlineStr"/>
       <c r="F12" s="20" t="n"/>
       <c r="G12" s="50" t="n"/>
       <c r="H12" s="156" t="n"/>
@@ -1894,11 +1842,11 @@
       <c r="R12" s="1" t="n"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="15" t="n"/>
-      <c r="B13" s="51" t="n"/>
-      <c r="C13" s="155" t="n"/>
+      <c r="A13" s="15" t="inlineStr"/>
+      <c r="B13" s="51" t="inlineStr"/>
+      <c r="C13" s="155" t="inlineStr"/>
       <c r="D13" s="151" t="n"/>
-      <c r="E13" s="64" t="n"/>
+      <c r="E13" s="64" t="inlineStr"/>
       <c r="F13" s="20" t="n"/>
       <c r="G13" s="50" t="n"/>
       <c r="H13" s="156" t="n"/>
@@ -1909,11 +1857,11 @@
       <c r="R13" s="1" t="n"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="15" t="n"/>
-      <c r="B14" s="51" t="n"/>
-      <c r="C14" s="150" t="n"/>
+      <c r="A14" s="15" t="inlineStr"/>
+      <c r="B14" s="51" t="inlineStr"/>
+      <c r="C14" s="150" t="inlineStr"/>
       <c r="D14" s="151" t="n"/>
-      <c r="E14" s="64" t="n"/>
+      <c r="E14" s="64" t="inlineStr"/>
       <c r="F14" s="21" t="n"/>
       <c r="G14" s="50" t="n"/>
       <c r="H14" s="154" t="n"/>
@@ -1924,11 +1872,11 @@
       <c r="R14" s="1" t="n"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="15" t="n"/>
-      <c r="B15" s="51" t="n"/>
-      <c r="C15" s="49" t="n"/>
+      <c r="A15" s="15" t="inlineStr"/>
+      <c r="B15" s="51" t="inlineStr"/>
+      <c r="C15" s="49" t="inlineStr"/>
       <c r="D15" s="151" t="n"/>
-      <c r="E15" s="64" t="n"/>
+      <c r="E15" s="64" t="inlineStr"/>
       <c r="F15" s="16" t="n"/>
       <c r="G15" s="50" t="n"/>
       <c r="H15" s="156" t="n"/>
@@ -1939,11 +1887,11 @@
       <c r="R15" s="1" t="n"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="15" t="n"/>
-      <c r="B16" s="51" t="n"/>
-      <c r="C16" s="49" t="n"/>
+      <c r="A16" s="15" t="inlineStr"/>
+      <c r="B16" s="51" t="inlineStr"/>
+      <c r="C16" s="49" t="inlineStr"/>
       <c r="D16" s="151" t="n"/>
-      <c r="E16" s="27" t="n"/>
+      <c r="E16" s="27" t="inlineStr"/>
       <c r="F16" s="16" t="n"/>
       <c r="G16" s="50" t="n"/>
       <c r="H16" s="156" t="n"/>
@@ -2058,21 +2006,11 @@
       <c r="P20" s="1" t="n"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="17" t="inlineStr">
-        <is>
-          <t>GL 501</t>
-        </is>
-      </c>
-      <c r="B21" s="51" t="inlineStr">
-        <is>
-          <t>10:15</t>
-        </is>
-      </c>
+      <c r="A21" s="17" t="inlineStr"/>
+      <c r="B21" s="51" t="inlineStr"/>
       <c r="C21" s="49" t="inlineStr"/>
       <c r="D21" s="151" t="n"/>
-      <c r="E21" s="29" t="n">
-        <v>0</v>
-      </c>
+      <c r="E21" s="29" t="inlineStr"/>
       <c r="F21" s="56" t="n"/>
       <c r="G21" s="50" t="n"/>
       <c r="H21" s="161" t="n"/>
@@ -2082,25 +2020,11 @@
       <c r="P21" s="1" t="n"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="49" t="inlineStr">
-        <is>
-          <t>GL 533</t>
-        </is>
-      </c>
-      <c r="B22" s="51" t="inlineStr">
-        <is>
-          <t>12:40</t>
-        </is>
-      </c>
-      <c r="C22" s="155" t="inlineStr">
-        <is>
-          <t>2;</t>
-        </is>
-      </c>
+      <c r="A22" s="49" t="inlineStr"/>
+      <c r="B22" s="51" t="inlineStr"/>
+      <c r="C22" s="155" t="inlineStr"/>
       <c r="D22" s="151" t="n"/>
-      <c r="E22" s="64" t="n">
-        <v>1</v>
-      </c>
+      <c r="E22" s="64" t="inlineStr"/>
       <c r="F22" s="57" t="n"/>
       <c r="G22" s="50" t="n"/>
       <c r="H22" s="163" t="n"/>
@@ -2110,25 +2034,11 @@
       <c r="Q22" s="1" t="n"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="49" t="inlineStr">
-        <is>
-          <t>GL 571</t>
-        </is>
-      </c>
-      <c r="B23" s="51" t="inlineStr">
-        <is>
-          <t>13:10</t>
-        </is>
-      </c>
-      <c r="C23" s="155" t="inlineStr">
-        <is>
-          <t>2;</t>
-        </is>
-      </c>
+      <c r="A23" s="49" t="inlineStr"/>
+      <c r="B23" s="51" t="inlineStr"/>
+      <c r="C23" s="155" t="inlineStr"/>
       <c r="D23" s="151" t="n"/>
-      <c r="E23" s="60" t="n">
-        <v>1</v>
-      </c>
+      <c r="E23" s="60" t="inlineStr"/>
       <c r="F23" s="58" t="n"/>
       <c r="G23" s="50" t="n"/>
       <c r="H23" s="156" t="n"/>
@@ -2137,11 +2047,11 @@
       <c r="P23" s="1" t="n"/>
     </row>
     <row r="24" ht="15" customHeight="1">
-      <c r="A24" s="18" t="n"/>
-      <c r="B24" s="51" t="n"/>
-      <c r="C24" s="155" t="n"/>
+      <c r="A24" s="18" t="inlineStr"/>
+      <c r="B24" s="51" t="inlineStr"/>
+      <c r="C24" s="155" t="inlineStr"/>
       <c r="D24" s="151" t="n"/>
-      <c r="E24" s="60" t="n"/>
+      <c r="E24" s="60" t="inlineStr"/>
       <c r="F24" s="20" t="n"/>
       <c r="G24" s="50" t="n"/>
       <c r="H24" s="156" t="n"/>
@@ -2151,11 +2061,11 @@
       <c r="N24" s="2" t="n"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="15" t="n"/>
-      <c r="B25" s="51" t="n"/>
-      <c r="C25" s="164" t="n"/>
+      <c r="A25" s="15" t="inlineStr"/>
+      <c r="B25" s="51" t="inlineStr"/>
+      <c r="C25" s="164" t="inlineStr"/>
       <c r="D25" s="151" t="n"/>
-      <c r="E25" s="60" t="n"/>
+      <c r="E25" s="60" t="inlineStr"/>
       <c r="F25" s="20" t="n"/>
       <c r="G25" s="50" t="n"/>
       <c r="H25" s="154" t="n"/>
@@ -2166,11 +2076,11 @@
       <c r="N25" s="2" t="n"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="17" t="n"/>
-      <c r="B26" s="51" t="n"/>
-      <c r="C26" s="150" t="n"/>
+      <c r="A26" s="17" t="inlineStr"/>
+      <c r="B26" s="51" t="inlineStr"/>
+      <c r="C26" s="150" t="inlineStr"/>
       <c r="D26" s="151" t="n"/>
-      <c r="E26" s="60" t="n"/>
+      <c r="E26" s="60" t="inlineStr"/>
       <c r="F26" s="21" t="n"/>
       <c r="G26" s="50" t="n"/>
       <c r="H26" s="154" t="n"/>
@@ -2181,11 +2091,11 @@
       <c r="N26" s="2" t="n"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="15" t="n"/>
-      <c r="B27" s="51" t="n"/>
-      <c r="C27" s="156" t="n"/>
+      <c r="A27" s="15" t="inlineStr"/>
+      <c r="B27" s="51" t="inlineStr"/>
+      <c r="C27" s="156" t="inlineStr"/>
       <c r="D27" s="151" t="n"/>
-      <c r="E27" s="60" t="n"/>
+      <c r="E27" s="60" t="inlineStr"/>
       <c r="F27" s="21" t="n"/>
       <c r="G27" s="50" t="n"/>
       <c r="H27" s="156" t="n"/>
@@ -2196,11 +2106,11 @@
       <c r="N27" s="2" t="n"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="18" t="n"/>
-      <c r="B28" s="59" t="n"/>
-      <c r="C28" s="156" t="n"/>
+      <c r="A28" s="18" t="inlineStr"/>
+      <c r="B28" s="59" t="inlineStr"/>
+      <c r="C28" s="156" t="inlineStr"/>
       <c r="D28" s="151" t="n"/>
-      <c r="E28" s="33" t="n"/>
+      <c r="E28" s="33" t="inlineStr"/>
       <c r="F28" s="21" t="n"/>
       <c r="G28" s="50" t="n"/>
       <c r="H28" s="93" t="n"/>
@@ -2211,11 +2121,11 @@
       <c r="N28" s="2" t="n"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="18" t="n"/>
-      <c r="B29" s="51" t="n"/>
-      <c r="C29" s="156" t="n"/>
+      <c r="A29" s="18" t="inlineStr"/>
+      <c r="B29" s="51" t="inlineStr"/>
+      <c r="C29" s="156" t="inlineStr"/>
       <c r="D29" s="151" t="n"/>
-      <c r="E29" s="33" t="n"/>
+      <c r="E29" s="33" t="inlineStr"/>
       <c r="F29" s="21" t="n"/>
       <c r="G29" s="50" t="n"/>
       <c r="H29" s="93" t="n"/>
@@ -2226,11 +2136,11 @@
       <c r="N29" s="2" t="n"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="18" t="n"/>
-      <c r="B30" s="51" t="n"/>
-      <c r="C30" s="49" t="n"/>
+      <c r="A30" s="18" t="inlineStr"/>
+      <c r="B30" s="51" t="inlineStr"/>
+      <c r="C30" s="49" t="inlineStr"/>
       <c r="D30" s="151" t="n"/>
-      <c r="E30" s="33" t="n"/>
+      <c r="E30" s="33" t="inlineStr"/>
       <c r="F30" s="34" t="n"/>
       <c r="G30" s="50" t="n"/>
       <c r="H30" s="156" t="n"/>
@@ -2241,11 +2151,11 @@
       <c r="N30" s="2" t="n"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="18" t="n"/>
-      <c r="B31" s="51" t="n"/>
-      <c r="C31" s="156" t="n"/>
+      <c r="A31" s="18" t="inlineStr"/>
+      <c r="B31" s="51" t="inlineStr"/>
+      <c r="C31" s="156" t="inlineStr"/>
       <c r="D31" s="151" t="n"/>
-      <c r="E31" s="33" t="n"/>
+      <c r="E31" s="33" t="inlineStr"/>
       <c r="F31" s="21" t="n"/>
       <c r="G31" s="50" t="n"/>
       <c r="H31" s="156" t="n"/>

</xml_diff>